<commit_message>
Added Music in TheLadder
</commit_message>
<xml_diff>
--- a/questionsFile.xlsx
+++ b/questionsFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erica\IdeaProjects\Let_OS_Play\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EzGhou\Desktop\Let_OS_Play_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9067808A-2853-4758-B3EB-B760816E7D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0014C433-91B3-465E-BA4E-D4B98B5ED2A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Theoretical" sheetId="3" r:id="rId1"/>
@@ -663,11 +663,6 @@
 from within the file which it is declared.</t>
   </si>
   <si>
-    <t>Allows programmers to think applications as sets of
-concurrent processes acting upon logically shared 
-data structures.</t>
-  </si>
-  <si>
     <t>Pure ____ programming disallows the use of side-effects,
 while _____  programming disallows the use of goto
 statement.</t>
@@ -856,6 +851,11 @@
   <si>
     <t>Allows writing smaller algorithms and operating by
 looking only at the inputs to a function.</t>
+  </si>
+  <si>
+    <t>Allows programmers to think applications as sets of 
+concurrent processes acting upon logically shared 
+data structures.</t>
   </si>
 </sst>
 </file>
@@ -1226,24 +1226,24 @@
   <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C5" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="12"/>
-    <col min="2" max="2" width="35.33203125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="12"/>
+    <col min="2" max="2" width="35.28515625" style="12" customWidth="1"/>
     <col min="3" max="3" width="105" style="12" customWidth="1"/>
     <col min="4" max="4" width="37" style="12" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" style="12" customWidth="1"/>
-    <col min="7" max="7" width="37.88671875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="34.88671875" style="12" customWidth="1"/>
-    <col min="9" max="9" width="18.109375" style="12" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="12"/>
+    <col min="5" max="5" width="32.7109375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="34.85546875" style="12" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" style="12" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>211</v>
+        <v>257</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -1301,7 +1301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>13</v>
@@ -1330,7 +1330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>9</v>
@@ -1359,7 +1359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>17</v>
@@ -1388,7 +1388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>21</v>
@@ -1417,7 +1417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>29</v>
@@ -1475,7 +1475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>41</v>
@@ -1562,7 +1562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
@@ -1591,7 +1591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>45</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>71</v>
@@ -1823,7 +1823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>45</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>47</v>
@@ -1852,7 +1852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>11</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>9</v>
@@ -1881,7 +1881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>11</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>81</v>
@@ -1968,7 +1968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>11</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>86</v>
@@ -2084,7 +2084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>11</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>78</v>
@@ -2113,7 +2113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>11</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>88</v>
@@ -2142,7 +2142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>9</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>90</v>
@@ -2171,7 +2171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>9</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>97</v>
@@ -2229,7 +2229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>9</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>105</v>
@@ -2287,7 +2287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>9</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>48</v>
@@ -2316,7 +2316,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>9</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>112</v>
@@ -2345,7 +2345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>9</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>114</v>
@@ -2374,7 +2374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>9</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>98</v>
@@ -2403,7 +2403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>121</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>121</v>
@@ -2461,7 +2461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>121</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>9</v>
@@ -2490,7 +2490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>121</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>122</v>
@@ -2519,7 +2519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>43</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>121</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D45" s="4" t="b">
         <v>1</v>
@@ -2548,7 +2548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>45</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>121</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D47" s="4" t="b">
         <v>1</v>
@@ -2606,7 +2606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>121</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>133</v>
@@ -2635,7 +2635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>47</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>121</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>136</v>
@@ -2664,7 +2664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>121</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>133</v>
@@ -2693,7 +2693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>49</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>121</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>136</v>
@@ -2722,7 +2722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>137</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>138</v>
@@ -2751,7 +2751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>51</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>137</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>141</v>
@@ -2780,7 +2780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>137</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>145</v>
@@ -2809,7 +2809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>53</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>137</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>145</v>
@@ -2838,7 +2838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>137</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>151</v>
@@ -2867,7 +2867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>55</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>137</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>145</v>
@@ -2896,7 +2896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>137</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>153</v>
@@ -2925,7 +2925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>57</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>59</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>137</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>164</v>
@@ -3012,7 +3012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>61</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>168</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>174</v>
@@ -3070,7 +3070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -3078,7 +3078,7 @@
         <v>168</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>178</v>
@@ -3099,7 +3099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>63</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>168</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>182</v>
@@ -3128,7 +3128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>168</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>179</v>
@@ -3157,7 +3157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>65</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>168</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>180</v>
@@ -3215,7 +3215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>67</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>168</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>194</v>
@@ -3244,7 +3244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>168</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>198</v>
@@ -3273,7 +3273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>69</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>168</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>201</v>

</xml_diff>